<commit_message>
Graph and cleaning tweaks
</commit_message>
<xml_diff>
--- a/data/old/test-data.3.xlsx
+++ b/data/old/test-data.3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kschaumberg/Library/CloudStorage/Dropbox/Code/BMIz_forecasting/TeenGrowth/data/old/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7297D8-370E-2243-8120-15FF2B44CD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB29EB6-56E6-9748-9C08-2D8A9C7B0C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="760" windowWidth="28040" windowHeight="16940" xr2:uid="{4A6836CC-669B-E546-B897-ED7B4933A935}"/>
+    <workbookView xWindow="2200" yWindow="760" windowWidth="28040" windowHeight="16940" xr2:uid="{4A6836CC-669B-E546-B897-ED7B4933A935}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="8">
   <si>
     <t>age</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>height</t>
   </si>
 </sst>
 </file>
@@ -408,453 +411,531 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CDC928B-9E2E-A849-A586-716F84CF136F}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:E26"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>5</v>
       </c>
       <c r="B2">
+        <v>40</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
       <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
         <v>64</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>6</v>
       </c>
       <c r="B3">
+        <v>44</v>
+      </c>
+      <c r="C3">
         <v>0.96</v>
       </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
       <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
         <v>64</v>
       </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>7.6</v>
       </c>
       <c r="B4">
+        <v>48</v>
+      </c>
+      <c r="C4">
         <v>0.6</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
       <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
         <v>64</v>
       </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>9.8000000000000007</v>
       </c>
       <c r="B5">
+        <v>50</v>
+      </c>
+      <c r="C5">
         <v>0.8</v>
       </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
       <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
         <v>64</v>
       </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>10</v>
       </c>
       <c r="B6">
+        <v>55</v>
+      </c>
+      <c r="C6">
         <v>0.8</v>
       </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
       <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
         <v>64</v>
       </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>11</v>
       </c>
       <c r="B7">
+        <v>58</v>
+      </c>
+      <c r="C7">
         <v>0.7</v>
       </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
       <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
         <v>64</v>
       </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>11.5</v>
       </c>
       <c r="B8">
+        <v>60</v>
+      </c>
+      <c r="C8">
         <v>1</v>
       </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
       <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
         <v>64</v>
       </c>
-      <c r="E8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>12</v>
       </c>
       <c r="B9">
+        <v>62</v>
+      </c>
+      <c r="C9">
         <v>0.4</v>
       </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
       <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
         <v>64</v>
       </c>
-      <c r="E9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>12.3</v>
       </c>
       <c r="B10">
+        <v>63</v>
+      </c>
+      <c r="C10">
         <v>-0.1</v>
       </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
       <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
         <v>64</v>
       </c>
-      <c r="E10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
       <c r="B11">
+        <v>36</v>
+      </c>
+      <c r="C11">
         <v>-0.6</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>2</v>
       </c>
-      <c r="D11">
-        <v>68</v>
-      </c>
-      <c r="E11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>68</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
       <c r="B12">
+        <v>41</v>
+      </c>
+      <c r="C12">
         <v>-0.7</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>2</v>
       </c>
-      <c r="D12">
-        <v>68</v>
-      </c>
-      <c r="E12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>68</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4.5</v>
       </c>
       <c r="B13">
+        <v>43</v>
+      </c>
+      <c r="C13">
         <v>-0.8</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>2</v>
       </c>
-      <c r="D13">
-        <v>68</v>
-      </c>
-      <c r="E13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>68</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>6</v>
       </c>
       <c r="B14">
+        <v>47</v>
+      </c>
+      <c r="C14">
         <v>-0.6</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>2</v>
       </c>
-      <c r="D14">
-        <v>68</v>
-      </c>
-      <c r="E14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>68</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>9.1</v>
       </c>
       <c r="B15">
+        <v>58</v>
+      </c>
+      <c r="C15">
         <v>-1.2</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>2</v>
       </c>
-      <c r="D15">
-        <v>68</v>
-      </c>
-      <c r="E15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>68</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>11</v>
       </c>
       <c r="B16">
+        <v>64</v>
+      </c>
+      <c r="C16">
         <v>-0.5</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>2</v>
       </c>
-      <c r="D16">
-        <v>68</v>
-      </c>
-      <c r="E16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>68</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
       <c r="B17">
+        <v>68</v>
+      </c>
+      <c r="C17">
         <v>-0.6</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>2</v>
       </c>
-      <c r="D17">
-        <v>68</v>
-      </c>
-      <c r="E17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>68</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>14.5</v>
       </c>
       <c r="B18">
+        <v>68</v>
+      </c>
+      <c r="C18">
         <v>-0.3</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>2</v>
       </c>
-      <c r="D18">
-        <v>68</v>
-      </c>
-      <c r="E18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>68</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>15</v>
       </c>
       <c r="B19">
+        <v>68</v>
+      </c>
+      <c r="C19">
         <v>-1.5</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>2</v>
       </c>
-      <c r="D19">
-        <v>68</v>
-      </c>
-      <c r="E19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>68</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B20">
+        <v>48</v>
+      </c>
+      <c r="C20">
         <v>-0.1</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>70.2</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>5</v>
+        <v>7.6</v>
       </c>
       <c r="B21">
+        <v>50</v>
+      </c>
+      <c r="C21">
         <v>0</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>1</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>70.2</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>6.2</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="B22">
+        <v>51</v>
+      </c>
+      <c r="C22">
         <v>-0.25</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>1</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>70.2</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>7.2</v>
+        <v>10</v>
       </c>
       <c r="B23">
+        <v>56</v>
+      </c>
+      <c r="C23">
         <v>0.5</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>1</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>70.2</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B24">
+        <v>63</v>
+      </c>
+      <c r="C24">
         <v>0</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>1</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>70.2</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B25">
+        <v>66</v>
+      </c>
+      <c r="C25">
         <v>-1</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>1</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>70.2</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B26">
+        <v>70</v>
+      </c>
+      <c r="C26">
         <v>-1.5</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>1</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>70.2</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>